<commit_message>
started to save results to html per days
</commit_message>
<xml_diff>
--- a/Averages/averages.xlsx
+++ b/Averages/averages.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="14">
   <si>
     <t>city</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>Garage</t>
+  </si>
+  <si>
+    <t>Flat</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -794,6 +797,130 @@
         <v>798</v>
       </c>
     </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="2">
+        <v>43847</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>119.1052631578947</v>
+      </c>
+      <c r="E16">
+        <v>32676315.78947368</v>
+      </c>
+      <c r="F16">
+        <v>296798.3356605554</v>
+      </c>
+      <c r="G16">
+        <v>486.8421052631579</v>
+      </c>
+      <c r="H16">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="2">
+        <v>43847</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17">
+        <v>115.8809523809524</v>
+      </c>
+      <c r="E17">
+        <v>25552380.95238095</v>
+      </c>
+      <c r="F17">
+        <v>228041.7572974148</v>
+      </c>
+      <c r="G17">
+        <v>181.5</v>
+      </c>
+      <c r="H17">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="2">
+        <v>43847</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18">
+        <v>65.3952380952381</v>
+      </c>
+      <c r="E18">
+        <v>27610738.0952381</v>
+      </c>
+      <c r="F18">
+        <v>426755.1999621868</v>
+      </c>
+      <c r="H18">
+        <v>2520</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="2">
+        <v>43847</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19">
+        <v>17.75</v>
+      </c>
+      <c r="E19">
+        <v>4148100</v>
+      </c>
+      <c r="F19">
+        <v>240649.1567228772</v>
+      </c>
+      <c r="H19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="2">
+        <v>43847</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20">
+        <v>163.6563658838072</v>
+      </c>
+      <c r="E20">
+        <v>56148529.04820766</v>
+      </c>
+      <c r="F20">
+        <v>979818.0885652011</v>
+      </c>
+      <c r="G20">
+        <v>460.5908529048208</v>
+      </c>
+      <c r="H20">
+        <v>809</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
21st jan 2020 run
</commit_message>
<xml_diff>
--- a/Averages/averages.xlsx
+++ b/Averages/averages.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="14">
   <si>
     <t>city</t>
   </si>
@@ -419,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -921,6 +921,130 @@
         <v>809</v>
       </c>
     </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="2">
+        <v>43851</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21">
+        <v>116.2941176470588</v>
+      </c>
+      <c r="E21">
+        <v>32385294.11764706</v>
+      </c>
+      <c r="F21">
+        <v>296691.8471062569</v>
+      </c>
+      <c r="G21">
+        <v>468</v>
+      </c>
+      <c r="H21">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="2">
+        <v>43851</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22">
+        <v>103.9</v>
+      </c>
+      <c r="E22">
+        <v>23926000</v>
+      </c>
+      <c r="F22">
+        <v>232894.34794284</v>
+      </c>
+      <c r="G22">
+        <v>179.0333333333333</v>
+      </c>
+      <c r="H22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="2">
+        <v>43851</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23">
+        <v>65.48168892718655</v>
+      </c>
+      <c r="E23">
+        <v>27897462.30073244</v>
+      </c>
+      <c r="F23">
+        <v>429922.6476606705</v>
+      </c>
+      <c r="H23">
+        <v>2321</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="2">
+        <v>43851</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24">
+        <v>17.88607594936709</v>
+      </c>
+      <c r="E24">
+        <v>4128101.265822785</v>
+      </c>
+      <c r="F24">
+        <v>239682.3778796598</v>
+      </c>
+      <c r="H24">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="2">
+        <v>43851</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25">
+        <v>166.7172413793103</v>
+      </c>
+      <c r="E25">
+        <v>58262137.93103448</v>
+      </c>
+      <c r="F25">
+        <v>1062076.207434499</v>
+      </c>
+      <c r="G25">
+        <v>458.5724137931035</v>
+      </c>
+      <c r="H25">
+        <v>725</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed the way we extract the size and land size. Now it understands if there is a space in the text
</commit_message>
<xml_diff>
--- a/Averages/averages.xlsx
+++ b/Averages/averages.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="14">
   <si>
     <t>city</t>
   </si>
@@ -419,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1665,6 +1665,130 @@
         <v>835</v>
       </c>
     </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="2">
+        <v>43893</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51">
+        <v>113.8095238095238</v>
+      </c>
+      <c r="E51">
+        <v>31133333.33333333</v>
+      </c>
+      <c r="F51">
+        <v>287581.7671387243</v>
+      </c>
+      <c r="G51">
+        <v>464.8095238095238</v>
+      </c>
+      <c r="H51">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="2">
+        <v>43893</v>
+      </c>
+      <c r="B52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52">
+        <v>122.4047619047619</v>
+      </c>
+      <c r="E52">
+        <v>30370238.0952381</v>
+      </c>
+      <c r="F52">
+        <v>251363.0346858636</v>
+      </c>
+      <c r="G52">
+        <v>153.3333333333333</v>
+      </c>
+      <c r="H52">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="2">
+        <v>43893</v>
+      </c>
+      <c r="B53" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53">
+        <v>65.29819277108433</v>
+      </c>
+      <c r="E53">
+        <v>27861588.85542169</v>
+      </c>
+      <c r="F53">
+        <v>431660.3488087555</v>
+      </c>
+      <c r="H53">
+        <v>2656</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="2">
+        <v>43893</v>
+      </c>
+      <c r="B54" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54">
+        <v>17.68965517241379</v>
+      </c>
+      <c r="E54">
+        <v>3981839.08045977</v>
+      </c>
+      <c r="F54">
+        <v>233766.3635384706</v>
+      </c>
+      <c r="H54">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="2">
+        <v>43893</v>
+      </c>
+      <c r="B55" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55">
+        <v>162.2271062271062</v>
+      </c>
+      <c r="E55">
+        <v>56672832.72283272</v>
+      </c>
+      <c r="F55">
+        <v>974787.8027311168</v>
+      </c>
+      <c r="G55">
+        <v>466.4029304029304</v>
+      </c>
+      <c r="H55">
+        <v>819</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>